<commit_message>
new PKGCONFIGS; new tools in DB; Update xlsx
</commit_message>
<xml_diff>
--- a/package_status.xlsx
+++ b/package_status.xlsx
@@ -76,9 +76,6 @@
     <t>hashid</t>
   </si>
   <si>
-    <t>precisa mudar nome do arquivo</t>
-  </si>
-  <si>
     <t>hydra</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>john</t>
+  </si>
+  <si>
+    <t>sem instalação</t>
   </si>
   <si>
     <t>linset</t>
@@ -157,9 +157,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -178,8 +178,130 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -199,128 +321,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -331,91 +331,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,91 +511,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,35 +525,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -569,17 +551,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,6 +572,26 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -608,17 +599,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,145 +627,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1096,8 +1096,8 @@
   <sheetPr/>
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -1180,7 +1180,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -1211,7 +1211,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1220,7 +1220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1232,6 +1232,9 @@
       </c>
       <c r="D8" t="s">
         <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1276,7 +1279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1292,13 +1295,10 @@
       <c r="E12" t="s">
         <v>13</v>
       </c>
-      <c r="H12" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -1327,18 +1327,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1346,7 +1349,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -1411,7 +1414,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1423,6 +1426,9 @@
       </c>
       <c r="D21" t="s">
         <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:4">

</xml_diff>

<commit_message>
update wpscan; added xssya
</commit_message>
<xml_diff>
--- a/package_status.xlsx
+++ b/package_status.xlsx
@@ -168,10 +168,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -190,6 +190,104 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -198,32 +296,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -236,105 +333,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,55 +343,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,127 +493,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,17 +543,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -567,11 +576,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,20 +606,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,17 +632,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,157 +645,163 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1108,8 +1120,8 @@
   <sheetPr/>
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -1160,7 +1172,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -1188,7 +1200,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
@@ -1232,7 +1244,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1244,6 +1256,9 @@
       </c>
       <c r="D8" t="s">
         <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1278,7 +1293,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
@@ -1323,7 +1338,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="s">
@@ -1402,7 +1417,7 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B19" t="s">
@@ -1534,7 +1549,7 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B28" t="s">
@@ -1548,7 +1563,7 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B29" t="s">
@@ -1562,7 +1577,7 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B30" t="s">
@@ -1593,7 +1608,7 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B32" t="s">
@@ -1621,7 +1636,7 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B34" t="s">
@@ -1655,7 +1670,7 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B36" t="s">
@@ -1669,11 +1684,11 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
         <v>9</v>
@@ -1683,7 +1698,7 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B38" t="s">

</xml_diff>

<commit_message>
updade xls; update author gen_pkgconfig.py
</commit_message>
<xml_diff>
--- a/package_status.xlsx
+++ b/package_status.xlsx
@@ -180,10 +180,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -207,16 +207,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -224,10 +216,17 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -239,10 +238,26 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -253,8 +268,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,22 +286,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,29 +313,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -337,17 +337,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -366,187 +366,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,6 +571,26 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,15 +634,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -661,164 +672,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1167,8 +1167,8 @@
   <sheetPr/>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -2110,20 +2110,20 @@
       <c r="K33" s="6"/>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
t50 ready to install
</commit_message>
<xml_diff>
--- a/package_status.xlsx
+++ b/package_status.xlsx
@@ -70,13 +70,13 @@
     <t>aircrack-ng</t>
   </si>
   <si>
+    <t>ok</t>
+  </si>
+  <si>
     <t>beef</t>
   </si>
   <si>
     <t>bully</t>
-  </si>
-  <si>
-    <t>ok</t>
   </si>
   <si>
     <t>cangibrina</t>
@@ -199,8 +199,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="30">
@@ -285,6 +285,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -293,6 +301,119 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -302,128 +423,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -438,187 +438,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -663,58 +663,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -753,7 +703,57 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -762,148 +762,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1264,8 +1264,8 @@
   <sheetPr/>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -1455,13 +1455,15 @@
         <v>13</v>
       </c>
       <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+      <c r="L5" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="M5" s="10"/>
       <c r="N5" s="12"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>13</v>
@@ -1497,7 +1499,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>12</v>
@@ -1528,7 +1530,7 @@
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="12"/>
@@ -1565,10 +1567,10 @@
         <v>13</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="12"/>
@@ -1605,10 +1607,10 @@
         <v>13</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="12"/>
@@ -1645,10 +1647,10 @@
         <v>13</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="12"/>
@@ -1793,10 +1795,10 @@
         <v>13</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="12"/>
@@ -1869,10 +1871,10 @@
         <v>13</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="12"/>
@@ -1947,10 +1949,10 @@
         <v>13</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="12"/>
@@ -1987,10 +1989,10 @@
         <v>13</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="12"/>
@@ -2063,10 +2065,10 @@
         <v>13</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="12"/>
@@ -2103,10 +2105,10 @@
         <v>13</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="12" t="s">
@@ -2187,10 +2189,10 @@
         <v>13</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="12"/>
@@ -2227,10 +2229,10 @@
         <v>13</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="12" t="s">
@@ -2491,10 +2493,10 @@
         <v>13</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L32" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="12"/>
@@ -2567,7 +2569,9 @@
         <v>13</v>
       </c>
       <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
+      <c r="L34" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="M34" s="10"/>
       <c r="N34" s="12"/>
     </row>
@@ -2639,7 +2643,7 @@
         <v>13</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>

</xml_diff>

<commit_message>
vega ready on arch
</commit_message>
<xml_diff>
--- a/package_status.xlsx
+++ b/package_status.xlsx
@@ -198,10 +198,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -294,10 +294,17 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -310,7 +317,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -325,23 +348,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -354,16 +362,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -377,8 +384,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -388,6 +403,21 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -398,36 +428,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -438,19 +438,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -462,157 +606,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,22 +664,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -699,11 +684,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -734,6 +725,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -748,117 +757,108 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -867,40 +867,40 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1264,8 +1264,8 @@
   <sheetPr/>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -1275,7 +1275,7 @@
     <col min="11" max="11" width="7.1" style="2" customWidth="1"/>
     <col min="12" max="12" width="7.3" style="2" customWidth="1"/>
     <col min="13" max="13" width="7.2" style="2" customWidth="1"/>
-    <col min="14" max="14" width="19.8" style="2" customWidth="1"/>
+    <col min="14" max="14" width="21.9" style="2" customWidth="1"/>
     <col min="15" max="16384" width="8.8" style="2"/>
   </cols>
   <sheetData>
@@ -2606,7 +2606,9 @@
       <c r="J35" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="10"/>
+      <c r="K35" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="N35" s="12"/>

</xml_diff>

<commit_message>
Create PKGCONFIG, move to its directories and add to DB automaticly
</commit_message>
<xml_diff>
--- a/package_status.xlsx
+++ b/package_status.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
   <si>
     <t>package</t>
   </si>
@@ -91,6 +91,9 @@
     <t>dnsenum</t>
   </si>
   <si>
+    <t>taking too long</t>
+  </si>
+  <si>
     <t>ettercap</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
     <t>hydra</t>
   </si>
   <si>
+    <t>can't find libnpc-dev</t>
+  </si>
+  <si>
     <t>inurlbr</t>
   </si>
   <si>
@@ -146,9 +152,6 @@
   </si>
   <si>
     <t>pompem</t>
-  </si>
-  <si>
-    <t>requirements erro</t>
   </si>
   <si>
     <t>proxychains</t>
@@ -198,10 +201,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -294,7 +297,23 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -303,6 +322,37 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -317,23 +367,43 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -341,7 +411,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,74 +426,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -438,13 +441,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,7 +525,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -468,157 +621,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,6 +659,21 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -699,17 +717,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -725,34 +746,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -762,145 +765,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1264,8 +1267,8 @@
   <sheetPr/>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -1689,11 +1692,13 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="12"/>
+      <c r="N11" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>12</v>
@@ -1729,7 +1734,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>13</v>
@@ -1765,7 +1770,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>12</v>
@@ -1805,7 +1810,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>12</v>
@@ -1837,11 +1842,13 @@
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="12"/>
+      <c r="N15" s="12" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>12</v>
@@ -1881,7 +1888,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>12</v>
@@ -1914,12 +1921,12 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>12</v>
@@ -1959,7 +1966,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>12</v>
@@ -1999,7 +2006,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>13</v>
@@ -2035,7 +2042,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>12</v>
@@ -2075,7 +2082,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>12</v>
@@ -2112,12 +2119,12 @@
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>12</v>
@@ -2154,12 +2161,12 @@
       </c>
       <c r="M23" s="10"/>
       <c r="N23" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>12</v>
@@ -2199,7 +2206,7 @@
     </row>
     <row r="25" spans="1:14">
       <c r="A25" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>12</v>
@@ -2236,12 +2243,12 @@
       </c>
       <c r="M25" s="10"/>
       <c r="N25" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>12</v>
@@ -2271,19 +2278,17 @@
         <v>13</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M26" s="10"/>
-      <c r="N26" s="12" t="s">
-        <v>43</v>
-      </c>
+      <c r="N26" s="12"/>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>13</v>
@@ -2319,7 +2324,7 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>13</v>
@@ -2355,7 +2360,7 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>13</v>
@@ -2391,7 +2396,7 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>13</v>
@@ -2427,7 +2432,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>12</v>
@@ -2463,7 +2468,7 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>12</v>
@@ -2503,7 +2508,7 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>13</v>
@@ -2539,7 +2544,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>12</v>
@@ -2577,7 +2582,7 @@
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>12</v>
@@ -2615,7 +2620,7 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>12</v>
@@ -2653,7 +2658,7 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>12</v>
@@ -2689,7 +2694,7 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>12</v>
@@ -2725,7 +2730,7 @@
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>13</v>
@@ -2761,7 +2766,7 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>13</v>

</xml_diff>